<commit_message>
COMPONENT DISTANCE AND BOARDOUTLINE ROOLS ACTIVATED,
</commit_message>
<xml_diff>
--- a/bom/PartsList.xlsx
+++ b/bom/PartsList.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="PartsList" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Quantity</t>
   </si>
@@ -42,7 +42,7 @@
     <t>CAPACITOR</t>
   </si>
   <si>
-    <t>0603_cap</t>
+    <t>0603_CAP_SMALL</t>
   </si>
   <si>
     <t>C1, C4, C5</t>
@@ -63,9 +63,6 @@
     <t>1uF/MLCC</t>
   </si>
   <si>
-    <t>0603_CAP</t>
-  </si>
-  <si>
     <t>C8, C10</t>
   </si>
   <si>
@@ -102,10 +99,10 @@
     <t>NSR20F30NXT5G</t>
   </si>
   <si>
-    <t>DIODE</t>
-  </si>
-  <si>
-    <t>0603_DIODE-CDSU101A</t>
+    <t>SCHOTTKY DIODE 0603</t>
+  </si>
+  <si>
+    <t>0603_DIODE-NSR20F30</t>
   </si>
   <si>
     <t>D5</t>
@@ -114,7 +111,7 @@
     <t>USB-MINI-B</t>
   </si>
   <si>
-    <t>USB-MINI-B-HIR-UX60A-MB-5ST</t>
+    <t>USB-MINI-B-HIR-UX60A-MB-5ST-SMALL</t>
   </si>
   <si>
     <t>JP2</t>
@@ -138,7 +135,7 @@
     <t>RESISTOR</t>
   </si>
   <si>
-    <t>0603_res</t>
+    <t>0603_res_SMALL</t>
   </si>
   <si>
     <t>R1, R3, R4, R9, R14</t>
@@ -225,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,9 +349,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -387,9 +384,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -575,11 +572,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="40" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,10 +658,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -672,16 +669,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,16 +686,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -706,16 +703,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -723,16 +720,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -740,16 +737,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -757,16 +754,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -774,16 +771,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -791,16 +788,16 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -808,16 +805,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -825,16 +822,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -842,16 +839,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -859,16 +856,16 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -876,16 +873,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -893,16 +890,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -910,16 +907,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -927,16 +924,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -944,20 +941,20 @@
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>